<commit_message>
created methods for checking if labels, types, and units exist in a sheet with paired data
added path to small-pd.xlsx

finished making ExcelReader paired data tests
</commit_message>
<xml_diff>
--- a/DSSExcelTests/test-files/small-pd.xlsx
+++ b/DSSExcelTests/test-files/small-pd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DSSExcelPlugin\DSSExcelTests\test-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A64364E-B288-48B1-9518-80635278A225}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC02278-0816-41AF-87A6-F4F7C18606E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="405" windowWidth="15330" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75" yWindow="345" windowWidth="15330" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Xordinate</t>
   </si>
@@ -37,6 +37,63 @@
   </si>
   <si>
     <t>Value 3</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Unit 1</t>
+  </si>
+  <si>
+    <t>Unit 2</t>
+  </si>
+  <si>
+    <t>Type 1</t>
+  </si>
+  <si>
+    <t>Type 2</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>u1</t>
+  </si>
+  <si>
+    <t>u2</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
   </si>
 </sst>
 </file>
@@ -354,123 +411,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B12">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C12">
         <v>20</v>
       </c>
-      <c r="D2">
+      <c r="D12">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B13">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="C13">
         <v>22</v>
       </c>
-      <c r="D3">
+      <c r="D13">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B14">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C14">
         <v>24</v>
       </c>
-      <c r="D4">
+      <c r="D14">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B15">
         <v>13</v>
       </c>
-      <c r="C5">
+      <c r="C15">
         <v>26</v>
       </c>
-      <c r="D5">
+      <c r="D15">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B16">
         <v>14</v>
       </c>
-      <c r="C6">
+      <c r="C16">
         <v>28</v>
       </c>
-      <c r="D6">
+      <c r="D16">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>12</v>
       </c>
-      <c r="B7">
+      <c r="B17">
         <v>15</v>
       </c>
-      <c r="C7">
+      <c r="C17">
         <v>30</v>
       </c>
-      <c r="D7">
+      <c r="D17">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>14</v>
       </c>
-      <c r="B8">
+      <c r="B18">
         <v>16</v>
       </c>
-      <c r="C8">
+      <c r="C18">
         <v>32</v>
       </c>
-      <c r="D8">
+      <c r="D18">
         <v>48</v>
       </c>
     </row>

</xml_diff>